<commit_message>
Fiksa en del på plots
</commit_message>
<xml_diff>
--- a/Spot_Price_Results.xlsx
+++ b/Spot_Price_Results.xlsx
@@ -19,34 +19,34 @@
     <t>Hour</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>Price [NOK/kWh]</t>
   </si>
   <si>
-    <t>Demand</t>
+    <t>Demand [kW]</t>
   </si>
   <si>
-    <t>EV Demand</t>
+    <t>EV Demand [kW]</t>
   </si>
   <si>
-    <t>Battery SOC</t>
+    <t>Battery SOC [kWh]</t>
   </si>
   <si>
-    <t>Charge Power</t>
+    <t>Charge Power [kW]</t>
   </si>
   <si>
-    <t>Discharge Power</t>
+    <t>Discharge Power [kW]</t>
   </si>
   <si>
-    <t>EV SOC</t>
+    <t>EV SOC [kWh]</t>
   </si>
   <si>
-    <t>EV Charge Power</t>
+    <t>EV Charge Power [kW]</t>
   </si>
   <si>
-    <t>EV Discharge Power</t>
+    <t>EV Discharge Power [kW]</t>
   </si>
   <si>
-    <t>Power Import</t>
+    <t>Power Import [kW]</t>
   </si>
   <si>
     <t>ENS</t>

</xml_diff>

<commit_message>
Lagt inn insentivbasert ish
</commit_message>
<xml_diff>
--- a/Spot_Price_Results.xlsx
+++ b/Spot_Price_Results.xlsx
@@ -4777,10 +4777,10 @@
         <v>8.699999999999999</v>
       </c>
       <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
         <v>40.54958333333334</v>
-      </c>
-      <c r="L115">
-        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:12">
@@ -11751,13 +11751,13 @@
         <v>1.25</v>
       </c>
       <c r="E299">
-        <v>80</v>
+        <v>65.64102564102565</v>
       </c>
       <c r="F299">
         <v>0</v>
       </c>
       <c r="G299">
-        <v>0</v>
+        <v>13.99999999999999</v>
       </c>
       <c r="H299">
         <v>105.1</v>
@@ -11769,7 +11769,7 @@
         <v>0</v>
       </c>
       <c r="K299">
-        <v>51.08000000000001</v>
+        <v>37.08000000000001</v>
       </c>
       <c r="L299">
         <v>0</v>
@@ -11789,7 +11789,7 @@
         <v>1.35</v>
       </c>
       <c r="E300">
-        <v>63.58974358974359</v>
+        <v>49.23076923076924</v>
       </c>
       <c r="F300">
         <v>0</v>
@@ -11827,7 +11827,7 @@
         <v>2.025</v>
       </c>
       <c r="E301">
-        <v>63.58974358974359</v>
+        <v>49.23076923076924</v>
       </c>
       <c r="F301">
         <v>0</v>
@@ -11865,7 +11865,7 @@
         <v>2.75</v>
       </c>
       <c r="E302">
-        <v>63.58974358974359</v>
+        <v>49.23076923076924</v>
       </c>
       <c r="F302">
         <v>0</v>
@@ -11903,7 +11903,7 @@
         <v>3.975</v>
       </c>
       <c r="E303">
-        <v>63.58974358974359</v>
+        <v>49.23076923076924</v>
       </c>
       <c r="F303">
         <v>0</v>
@@ -11947,7 +11947,7 @@
         <v>0</v>
       </c>
       <c r="G304">
-        <v>13.99999999999999</v>
+        <v>0</v>
       </c>
       <c r="H304">
         <v>105.1</v>
@@ -11959,7 +11959,7 @@
         <v>0</v>
       </c>
       <c r="K304">
-        <v>28.28291666666668</v>
+        <v>42.28291666666667</v>
       </c>
       <c r="L304">
         <v>0</v>
@@ -25963,10 +25963,10 @@
         <v>6.1</v>
       </c>
       <c r="E673">
-        <v>2.000000000000002</v>
+        <v>15.6</v>
       </c>
       <c r="F673">
-        <v>2.051282051282053</v>
+        <v>16</v>
       </c>
       <c r="G673">
         <v>0</v>
@@ -25981,7 +25981,7 @@
         <v>0</v>
       </c>
       <c r="K673">
-        <v>60.94919871794872</v>
+        <v>74.89791666666667</v>
       </c>
       <c r="L673">
         <v>0</v>
@@ -26001,7 +26001,7 @@
         <v>5.774999999999999</v>
       </c>
       <c r="E674">
-        <v>17.6</v>
+        <v>31.2</v>
       </c>
       <c r="F674">
         <v>16</v>
@@ -26039,7 +26039,7 @@
         <v>4.074999999999999</v>
       </c>
       <c r="E675">
-        <v>33.2</v>
+        <v>46.8</v>
       </c>
       <c r="F675">
         <v>16</v>
@@ -26077,7 +26077,7 @@
         <v>2.774999999999999</v>
       </c>
       <c r="E676">
-        <v>48.8</v>
+        <v>62.4</v>
       </c>
       <c r="F676">
         <v>16</v>
@@ -26115,7 +26115,7 @@
         <v>1.85</v>
       </c>
       <c r="E677">
-        <v>64.40000000000001</v>
+        <v>78</v>
       </c>
       <c r="F677">
         <v>16</v>
@@ -26156,7 +26156,7 @@
         <v>80</v>
       </c>
       <c r="F678">
-        <v>16</v>
+        <v>2.051282051282052</v>
       </c>
       <c r="G678">
         <v>0</v>
@@ -26171,7 +26171,7 @@
         <v>0</v>
       </c>
       <c r="K678">
-        <v>43.6325</v>
+        <v>29.68378205128205</v>
       </c>
       <c r="L678">
         <v>0</v>

</xml_diff>